<commit_message>
Added 3 new capacitors.
</commit_message>
<xml_diff>
--- a/PCB/harp rfid reader BOM.xlsx
+++ b/PCB/harp rfid reader BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_RFID_reader\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13FE79E-7D7C-49CF-8E4C-DF7F66D7C67A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C31D68-1D97-44B7-B65F-A60F2902AEE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22DE42AE-D7DB-44FC-B9CF-DE1961A005DB}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>C0402</t>
   </si>
   <si>
-    <t>C7</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -216,15 +213,6 @@
     <t>04025A470JAT2A</t>
   </si>
   <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>A/3216-18W</t>
-  </si>
-  <si>
-    <t>TAJA475K016UNJ</t>
-  </si>
-  <si>
     <t>4.7nF</t>
   </si>
   <si>
@@ -318,9 +306,6 @@
     <t>541-1.00KLDKR-ND</t>
   </si>
   <si>
-    <t>478-11461-6-ND</t>
-  </si>
-  <si>
     <t>732-12234-6-ND</t>
   </si>
   <si>
@@ -381,9 +366,6 @@
     <t>C3, C4</t>
   </si>
   <si>
-    <t>C5, C11, C17</t>
-  </si>
-  <si>
     <t>C2, C6, C8, C9, C10, C12, C13, C14, C15, C16</t>
   </si>
   <si>
@@ -466,6 +448,24 @@
   </si>
   <si>
     <t>ATXMEGA32A4U-AUR</t>
+  </si>
+  <si>
+    <t>CT3216</t>
+  </si>
+  <si>
+    <t>298W107X0010Q2D</t>
+  </si>
+  <si>
+    <t>718-298W107X0010Q2DDKR-ND</t>
+  </si>
+  <si>
+    <t>100uF 20% 10V</t>
+  </si>
+  <si>
+    <t>C5, C7, C11, C17</t>
+  </si>
+  <si>
+    <t>C18, C19, C20</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1436,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23:I24"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,10 +1471,10 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1494,25 +1494,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1520,25 +1520,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1546,51 +1546,51 @@
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1598,25 +1598,25 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1624,26 +1624,26 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1651,25 +1651,25 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1677,25 +1677,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1703,25 +1703,25 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1729,25 +1729,25 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1755,25 +1755,25 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1781,25 +1781,25 @@
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1807,25 +1807,25 @@
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1833,25 +1833,25 @@
         <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1859,23 +1859,23 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1883,25 +1883,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1909,25 +1909,25 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1935,25 +1935,25 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1961,25 +1961,25 @@
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>28</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>29</v>
       </c>
       <c r="F21" s="21" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1987,23 +1987,23 @@
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2011,23 +2011,23 @@
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2035,23 +2035,23 @@
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2059,25 +2059,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2097,21 +2097,21 @@
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I27" s="18"/>
     </row>
@@ -2120,7 +2120,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2128,13 +2128,13 @@
         <v>887328502</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2194,18 +2194,18 @@
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E36" s="15" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F36" s="16">
         <v>49.74</v>
       </c>
       <c r="G36" s="19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F37" s="16">
         <v>29.95</v>
@@ -2214,7 +2214,7 @@
     <row r="38" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D38" s="14"/>
       <c r="E38" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F38" s="16">
         <v>8.9700000000000006</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F39" s="16">
         <v>2.2000000000000002</v>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F40" s="16">
         <v>12.5</v>
@@ -2238,7 +2238,7 @@
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F41" s="16">
         <v>0.27</v>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E42" s="17" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F42" s="16">
         <f>SUM(F36:F41)</f>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E43" s="17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F43" s="16">
         <f>F42*2</f>

</xml_diff>

<commit_message>
Corrected STATE and DETECT lines and increased LED resistors.
</commit_message>
<xml_diff>
--- a/PCB/harp rfid reader BOM.xlsx
+++ b/PCB/harp rfid reader BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_RFID_reader\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C31D68-1D97-44B7-B65F-A60F2902AEE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDD0727-227B-473D-B8A6-404CFE60D91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22DE42AE-D7DB-44FC-B9CF-DE1961A005DB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22DE42AE-D7DB-44FC-B9CF-DE1961A005DB}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
   <si>
     <t>Qty</t>
   </si>
@@ -90,9 +90,6 @@
     <t>SMD</t>
   </si>
   <si>
-    <t>TH</t>
-  </si>
-  <si>
     <t>ASSEMBLY HOUSE</t>
   </si>
   <si>
@@ -162,18 +159,6 @@
     <t>445-6899-6-ND</t>
   </si>
   <si>
-    <t>910 1/10W 5%</t>
-  </si>
-  <si>
-    <t>RK73B1ETTP911J</t>
-  </si>
-  <si>
-    <t>2019-RK73B1ETTP911JDKR-ND</t>
-  </si>
-  <si>
-    <t>R2, R3, R4</t>
-  </si>
-  <si>
     <t>RED LED</t>
   </si>
   <si>
@@ -237,18 +222,6 @@
     <t>668-1060-6-ND</t>
   </si>
   <si>
-    <t>PDI</t>
-  </si>
-  <si>
-    <t>67996-206HLF</t>
-  </si>
-  <si>
-    <t>PROG HEADER</t>
-  </si>
-  <si>
-    <t>HEADER_3x2</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -360,9 +333,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>C3, C4</t>
   </si>
   <si>
@@ -390,9 +360,6 @@
     <t xml:space="preserve">Total </t>
   </si>
   <si>
-    <t>x2</t>
-  </si>
-  <si>
     <t>Assembly</t>
   </si>
   <si>
@@ -466,6 +433,9 @@
   </si>
   <si>
     <t>C18, C19, C20</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R6</t>
   </si>
 </sst>
 </file>
@@ -1433,11 +1403,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1471,15 +1439,15 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1494,25 +1462,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1520,25 +1488,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1546,25 +1514,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1572,25 +1540,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1598,25 +1566,25 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1624,52 +1592,52 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1677,25 +1645,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1703,25 +1671,25 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1729,25 +1697,25 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1755,25 +1723,25 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1781,491 +1749,434 @@
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="D17" s="4" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>128</v>
+        <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>105</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+    </row>
+    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>61</v>
+        <v>94</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-    </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+        <v>89</v>
+      </c>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>1</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="22">
+        <v>887328502</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="E28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="1">
+        <v>20</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="E29" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1">
+        <v>37</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E31" s="8"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="10"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E32" s="12"/>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E34" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="16">
+        <v>49.74</v>
+      </c>
+      <c r="G34" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H27" s="4" t="s">
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="16">
+        <v>29.95</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D36" s="14"/>
+      <c r="E36" t="s">
         <v>98</v>
       </c>
-      <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>1</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="22">
-        <v>887328502</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-    </row>
-    <row r="30" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="E30" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="1">
-        <v>22</v>
-      </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="E31" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="1">
-        <v>37</v>
-      </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-      <c r="H32" s="14"/>
-    </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E33" s="8"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E34" s="12"/>
-    </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E36" s="15" t="s">
-        <v>118</v>
-      </c>
       <c r="F36" s="16">
-        <v>49.74</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+        <v>8.9700000000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>99</v>
       </c>
       <c r="F37" s="16">
-        <v>29.95</v>
-      </c>
-    </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D38" s="14"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F38" s="16">
-        <v>8.9700000000000006</v>
-      </c>
-    </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F39" s="16">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
-        <v>112</v>
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="F40" s="16">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
-        <v>113</v>
-      </c>
-      <c r="F41" s="16">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E42" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="F42" s="16">
-        <f>SUM(F36:F41)</f>
+        <f>SUM(F34:F39)</f>
         <v>103.63</v>
       </c>
     </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E43" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="F43" s="16">
-        <f>F42*2</f>
-        <v>207.26</v>
-      </c>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="17"/>
+      <c r="F41" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A27:H27"/>
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added a digital output.
</commit_message>
<xml_diff>
--- a/PCB/harp rfid reader BOM.xlsx
+++ b/PCB/harp rfid reader BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_RFID_reader\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDD0727-227B-473D-B8A6-404CFE60D91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655EDBB1-A8B9-4583-A95E-977081D0B802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22DE42AE-D7DB-44FC-B9CF-DE1961A005DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22DE42AE-D7DB-44FC-B9CF-DE1961A005DB}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="131">
   <si>
     <t>Qty</t>
   </si>
@@ -171,9 +171,6 @@
     <t>350-2950-6-ND</t>
   </si>
   <si>
-    <t>TAG_B, TAG_T. STATE</t>
-  </si>
-  <si>
     <t>LP5907MFX-3.3/NOPB</t>
   </si>
   <si>
@@ -336,9 +333,6 @@
     <t>C3, C4</t>
   </si>
   <si>
-    <t>C2, C6, C8, C9, C10, C12, C13, C14, C15, C16</t>
-  </si>
-  <si>
     <t>RFID Reader ID-12LA (125 kHz)</t>
   </si>
   <si>
@@ -393,9 +387,6 @@
     <t>541-10407-6-ND</t>
   </si>
   <si>
-    <t>Not sure yet</t>
-  </si>
-  <si>
     <t>NPPN051BFLD-RC‎</t>
   </si>
   <si>
@@ -435,7 +426,28 @@
     <t>C18, C19, C20</t>
   </si>
   <si>
-    <t>R2, R3, R4, R6</t>
+    <t>M74VHC1GT126DT1G</t>
+  </si>
+  <si>
+    <t>M74VHC1GT126DT1GOSDKR-ND</t>
+  </si>
+  <si>
+    <t>IC4</t>
+  </si>
+  <si>
+    <t>TSOP-5</t>
+  </si>
+  <si>
+    <t>IC BUFFER NON-INVERT 5.5V</t>
+  </si>
+  <si>
+    <t>C2, C6, C8, C9, C10, C12, C13, C14, C15, C16, C21</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R6, R8</t>
+  </si>
+  <si>
+    <t>TAG_B, TAG_T, STATE, OUT0</t>
   </si>
 </sst>
 </file>
@@ -983,7 +995,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1015,7 +1027,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1032,9 +1043,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1403,9 +1411,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:H21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1419,7 +1429,7 @@
     <col min="8" max="8" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1445,33 +1455,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+    </row>
+    <row r="3" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>10</v>
@@ -1480,24 +1490,24 @@
         <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
@@ -1506,12 +1516,12 @@
         <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>32</v>
@@ -1520,7 +1530,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>20</v>
@@ -1535,18 +1545,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>21</v>
@@ -1558,24 +1568,24 @@
         <v>24</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>10</v>
@@ -1584,51 +1594,50 @@
         <v>24</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>1</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
+      <c r="F8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>10</v>
@@ -1637,10 +1646,10 @@
         <v>24</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -1651,10 +1660,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>10</v>
@@ -1663,15 +1672,15 @@
         <v>24</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>16</v>
@@ -1680,7 +1689,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>10</v>
@@ -1689,24 +1698,24 @@
         <v>24</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>10</v>
@@ -1715,24 +1724,24 @@
         <v>24</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>10</v>
@@ -1741,24 +1750,24 @@
         <v>24</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>10</v>
@@ -1767,12 +1776,12 @@
         <v>24</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>34</v>
@@ -1781,7 +1790,7 @@
         <v>35</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>36</v>
@@ -1796,19 +1805,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>10</v>
@@ -1817,24 +1826,24 @@
         <v>24</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>10</v>
@@ -1843,24 +1852,24 @@
         <v>24</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>10</v>
@@ -1869,15 +1878,15 @@
         <v>24</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>29</v>
@@ -1886,7 +1895,7 @@
         <v>31</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>10</v>
@@ -1895,48 +1904,50 @@
         <v>24</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="D21" s="4" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>10</v>
@@ -1945,22 +1956,22 @@
         <v>24</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>10</v>
@@ -1969,10 +1980,10 @@
         <v>24</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>1</v>
       </c>
@@ -1981,10 +1992,10 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>10</v>
@@ -1993,190 +2004,215 @@
         <v>24</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-    </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="22">
+      <c r="E26" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="21">
         <v>887328502</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F27" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G27" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="H27" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-    </row>
-    <row r="28" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="E28" s="14" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="E29" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="1">
-        <v>20</v>
-      </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="E29" s="14" t="s">
+      <c r="F29" s="1">
+        <v>21</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="E30" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="1">
-        <v>37</v>
-      </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14" t="s">
+      <c r="F30" s="1">
+        <v>41</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F31" s="1">
         <v>0</v>
       </c>
-      <c r="H30" s="14"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E31" s="8"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="10"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="12"/>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E34" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F34" s="16">
-        <v>49.74</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>104</v>
-      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="10"/>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="12"/>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
-        <v>90</v>
-      </c>
-      <c r="F35" s="16">
+      <c r="E35" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35" s="15">
+        <f>49.74+0.34+1.226</f>
+        <v>51.306000000000004</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="15">
         <v>29.95</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="14"/>
-      <c r="E36" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36" s="16">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D37" s="13"/>
+      <c r="E37" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="15">
         <v>8.9700000000000006</v>
-      </c>
-    </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E37" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" s="16">
-        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>101</v>
-      </c>
-      <c r="F38" s="16">
-        <v>12.5</v>
+        <v>97</v>
+      </c>
+      <c r="F38" s="15">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>102</v>
-      </c>
-      <c r="F39" s="16">
+        <v>99</v>
+      </c>
+      <c r="F39" s="15">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>100</v>
+      </c>
+      <c r="F40" s="15">
         <v>0.27</v>
       </c>
     </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E40" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F40" s="16">
-        <f>SUM(F34:F39)</f>
-        <v>103.63</v>
-      </c>
-    </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E41" s="17"/>
-      <c r="F41" s="16"/>
+      <c r="E41" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" s="15">
+        <f>SUM(F35:F40)</f>
+        <v>105.196</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="16"/>
+      <c r="F42" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A28:H28"/>
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added fabrication files and updated BOM.
</commit_message>
<xml_diff>
--- a/PCB/harp rfid reader BOM.xlsx
+++ b/PCB/harp rfid reader BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_RFID_reader\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655EDBB1-A8B9-4583-A95E-977081D0B802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B90C07D-58D5-4A24-A4B8-30AFD8626086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22DE42AE-D7DB-44FC-B9CF-DE1961A005DB}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="131">
   <si>
     <t>Qty</t>
   </si>
@@ -306,12 +306,6 @@
     <t>SOT-23-5</t>
   </si>
   <si>
-    <t>U1 5POS ROW</t>
-  </si>
-  <si>
-    <t>U1 7POS ROW</t>
-  </si>
-  <si>
     <t>CONN RCPT 7POS 0.1 GOLD SMD</t>
   </si>
   <si>
@@ -339,42 +333,15 @@
     <t>4-SMD</t>
   </si>
   <si>
-    <t>USB 2.0 Cable A Male to Mini B Male 0.8M</t>
-  </si>
-  <si>
     <t>541-10.0KLDKR-ND</t>
   </si>
   <si>
-    <t>PCB</t>
-  </si>
-  <si>
-    <t>USB cable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total </t>
-  </si>
-  <si>
-    <t>Assembly</t>
-  </si>
-  <si>
-    <t>Packaging</t>
-  </si>
-  <si>
-    <t>WM14083-ND</t>
-  </si>
-  <si>
-    <t>Components in digi-reel</t>
-  </si>
-  <si>
     <t>10uF 20% 16V X5R</t>
   </si>
   <si>
     <t>587-3238-6-ND</t>
   </si>
   <si>
-    <t>Components (if produce 10 units)</t>
-  </si>
-  <si>
     <t>39Ω 1/5watt 1% 0402</t>
   </si>
   <si>
@@ -448,6 +415,39 @@
   </si>
   <si>
     <t>TAG_B, TAG_T, STATE, OUT0</t>
+  </si>
+  <si>
+    <t>Check R7 value used</t>
+  </si>
+  <si>
+    <t>A98333-ND</t>
+  </si>
+  <si>
+    <t>282834-2</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>CONN Terminal block 2.54MM</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>PROG HEADER</t>
+  </si>
+  <si>
+    <t>PDI</t>
+  </si>
+  <si>
+    <t>67996-206HLF</t>
+  </si>
+  <si>
+    <t>U1 5POS</t>
+  </si>
+  <si>
+    <t>U1 7POS</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,13 +624,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -995,7 +988,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1004,45 +997,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1411,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:H21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1393,7 @@
     <col min="8" max="8" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1455,19 +1419,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="3" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1478,22 +1442,23 @@
         <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1506,20 +1471,21 @@
       <c r="D4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>11</v>
       </c>
@@ -1530,100 +1496,104 @@
         <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>1</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>106</v>
+      <c r="B8" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -1634,22 +1604,23 @@
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -1660,22 +1631,23 @@
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1</v>
       </c>
@@ -1688,20 +1660,21 @@
       <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1</v>
       </c>
@@ -1714,20 +1687,21 @@
       <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1</v>
       </c>
@@ -1740,20 +1714,21 @@
       <c r="D13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I13"/>
+    </row>
+    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -1766,20 +1741,21 @@
       <c r="D14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>4</v>
       </c>
@@ -1790,22 +1766,23 @@
         <v>35</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E15" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1</v>
       </c>
@@ -1816,20 +1793,21 @@
       <c r="D16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1</v>
       </c>
@@ -1842,20 +1820,21 @@
       <c r="D17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>1</v>
       </c>
@@ -1868,25 +1847,26 @@
       <c r="D18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>29</v>
@@ -1894,46 +1874,51 @@
       <c r="D19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="I19"/>
+    </row>
+    <row r="20" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="I20"/>
+      <c r="N20" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>1</v>
       </c>
@@ -1941,25 +1926,26 @@
         <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>1</v>
       </c>
@@ -1970,249 +1956,199 @@
       <c r="D22" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F23" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="D26" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I26"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>1</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="21">
-        <v>887328502</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="G28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-    </row>
-    <row r="29" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="E29" s="13" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="1">
-        <v>21</v>
-      </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="E30" s="13" t="s">
+      <c r="F30" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="1">
-        <v>41</v>
-      </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13" t="s">
+      <c r="F31" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="8"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E33" s="12"/>
-    </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E35" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" s="15">
-        <f>49.74+0.34+1.226</f>
-        <v>51.306000000000004</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
-        <v>89</v>
-      </c>
-      <c r="F36" s="15">
-        <v>29.95</v>
-      </c>
-    </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="13"/>
-      <c r="E37" t="s">
-        <v>96</v>
-      </c>
-      <c r="F37" s="15">
-        <v>8.9700000000000006</v>
-      </c>
-    </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
-        <v>97</v>
-      </c>
-      <c r="F38" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E39" t="s">
-        <v>99</v>
-      </c>
-      <c r="F39" s="15">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
-        <v>100</v>
-      </c>
-      <c r="F40" s="15">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E41" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F41" s="15">
-        <f>SUM(F35:F40)</f>
-        <v>105.196</v>
-      </c>
-    </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E42" s="16"/>
-      <c r="F42" s="15"/>
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="8"/>
+      <c r="F33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A29:H29"/>
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>